<commit_message>
Fix the test effects
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pooriya\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\Internet Engineering\Poject\Phase 1\Client-Side\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>کار</t>
   </si>
@@ -63,13 +66,31 @@
   </si>
   <si>
     <t>تنظیم Header و Footer در یک فایل جدا</t>
+  </si>
+  <si>
+    <t>صفحه ی ثبت نام و ورود به سیستم</t>
+  </si>
+  <si>
+    <t>توضیحات</t>
+  </si>
+  <si>
+    <t>پوریا</t>
+  </si>
+  <si>
+    <t>در Header وارد شده است. هر سه نوع را پذیرش می کند. تنها کافی است فیلدهای ثبت نام بازبینی و دقیقتر شوند.</t>
+  </si>
+  <si>
+    <t>پیدا کردن عکس مناسب با اندازه ی 1920*500 برای اسلایدر</t>
+  </si>
+  <si>
+    <t>ساخت Footer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,6 +110,11 @@
       <color theme="1"/>
       <name val="B Nazanin"/>
       <charset val="178"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="B Nazanin"/>
     </font>
   </fonts>
   <fills count="2">
@@ -111,17 +137,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="B Nazanin"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -151,17 +195,24 @@
     <dxf>
       <font>
         <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="B Nazanin"/>
-        <scheme val="none"/>
+        <i val="0"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -176,8 +227,28 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="B Nazanin"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="4"/>
+      <tableStyleElement type="headerRow" dxfId="3"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -190,11 +261,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B12" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3">
-  <autoFilter ref="A1:B12"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="کار" dataDxfId="0"/>
-    <tableColumn id="2" name="انجام دهنده" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C15" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:C15"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="کار" dataDxfId="2"/>
+    <tableColumn id="2" name="انجام دهنده" dataDxfId="0"/>
+    <tableColumn id="3" name="توضیحات" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -463,91 +535,135 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="84.33203125" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="81" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:3" ht="20.399999999999999">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18.600000000000001">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:2" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" s="4"/>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" ht="18.600000000000001">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:2" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" s="4"/>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" ht="18.600000000000001">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:2" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" s="4"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" ht="18.600000000000001">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:2" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="4"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" ht="18.600000000000001">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:2" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="4"/>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" ht="18.600000000000001">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:2" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" s="4"/>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" ht="18.600000000000001">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:2" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" s="4"/>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" ht="18.600000000000001">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:2" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="4"/>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" ht="18.600000000000001">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:2" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" s="4"/>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:3" ht="18.600000000000001">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:2" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:3" ht="18.600000000000001">
       <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="18.600000000000001">
+      <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" ht="18.600000000000001">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" ht="18.600000000000001">
+      <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Footer Fixed and Included!
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sarah\git\netProjectPhase1\UpWork\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\Internet Engineering\Poject\Phase 1\Client-Side\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9405"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -538,17 +538,17 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="84.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="84.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
     <col min="3" max="3" width="81" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21">
+    <row r="1" spans="1:3" ht="20.399999999999999">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -559,70 +559,70 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18.75">
+    <row r="2" spans="1:3" ht="18.600000000000001">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:3" ht="18.75">
+    <row r="3" spans="1:3" ht="18.600000000000001">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:3" ht="18.75">
+    <row r="4" spans="1:3" ht="18.600000000000001">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:3" ht="18.75">
+    <row r="5" spans="1:3" ht="18.600000000000001">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3" ht="18.75">
+    <row r="6" spans="1:3" ht="18.600000000000001">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:3" ht="18.75">
+    <row r="7" spans="1:3" ht="18.600000000000001">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:3" ht="18.75">
+    <row r="8" spans="1:3" ht="18.600000000000001">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3" ht="18.75">
+    <row r="9" spans="1:3" ht="18.600000000000001">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:3" ht="18.75">
+    <row r="10" spans="1:3" ht="18.600000000000001">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:3" ht="18.75">
+    <row r="11" spans="1:3" ht="18.600000000000001">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -631,7 +631,7 @@
       </c>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:3" ht="18.75">
+    <row r="12" spans="1:3" ht="18.600000000000001">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -642,7 +642,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="18.75">
+    <row r="13" spans="1:3" ht="18.600000000000001">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -651,14 +651,14 @@
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" ht="18.75">
+    <row r="14" spans="1:3" ht="18.600000000000001">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" ht="18.75">
+    <row r="15" spans="1:3" ht="18.600000000000001">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Index page Completed Even more!
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -538,7 +538,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Task List and change size and margin
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>کار</t>
   </si>
@@ -111,6 +111,21 @@
   </si>
   <si>
     <t>دورنما، مهارت ها، سوابق کاری، اطلاعات تماس و ...</t>
+  </si>
+  <si>
+    <t>تعریف در داشبورد کارجو</t>
+  </si>
+  <si>
+    <t>اضافه کردن این قابلیت در صفحه پروفایل شرکت</t>
+  </si>
+  <si>
+    <t>5تا عکس برای اسلایدر در نظر گرفته شد</t>
+  </si>
+  <si>
+    <t>تنظیم صفحات</t>
+  </si>
+  <si>
+    <t>تغییر سایز عنوان تب ها و تنظیم فاصله ها از اطراف</t>
   </si>
 </sst>
 </file>
@@ -164,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -172,6 +187,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -288,8 +306,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C15" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C16" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C16"/>
   <tableColumns count="3">
     <tableColumn id="1" name="کار" dataDxfId="2"/>
     <tableColumn id="2" name="انجام دهنده" dataDxfId="1"/>
@@ -562,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -634,15 +652,23 @@
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="3"/>
+      <c r="B6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="18.75">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="3"/>
+      <c r="B7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="18.75">
       <c r="A8" s="1" t="s">
@@ -670,8 +696,12 @@
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="3"/>
+      <c r="B10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="11" spans="1:3" ht="18.75">
       <c r="A11" s="1" t="s">
@@ -713,7 +743,9 @@
       <c r="B14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="15" spans="1:3" ht="18.75">
       <c r="A15" s="1" t="s">
@@ -722,6 +754,17 @@
       <c r="B15" s="4"/>
       <c r="C15" s="3" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75">
+      <c r="A16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>